<commit_message>
Minor dataset queries cleanup
</commit_message>
<xml_diff>
--- a/dataset/dataset_clean.xlsx
+++ b/dataset/dataset_clean.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\micha\homeworks\NLP\AgentToBeNamed\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\micha\homeworks\NLP\AgentToBeNamed\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066EE834-F3F8-44AD-A7E3-49256B2CA2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68A2FB7-DD5C-45F3-BBE2-C000CB632E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{51F2586A-075B-4256-83EE-790A211770F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="109">
   <si>
     <t>table_name</t>
   </si>
@@ -107,15 +107,6 @@
     <t>Is there a correlation between higher temperatures and shorter reaction times?</t>
   </si>
   <si>
-    <t>Determine the pH level range most commonly observed across all experiments.</t>
-  </si>
-  <si>
-    <t>is there a relationship between concentration and yield? Do higher concentrations tend to result in higher yields?</t>
-  </si>
-  <si>
-    <t>Create a scatter plot to visualize the relationship between temperature and reaction time.</t>
-  </si>
-  <si>
     <t>Analyze the correlation between volume and concentration levels in the experiments.</t>
   </si>
   <si>
@@ -140,9 +131,6 @@
     <t>correlation between blood pressure and heart rate</t>
   </si>
   <si>
-    <t>is there any patient with nausea side effect? Reply Yes or No.</t>
-  </si>
-  <si>
     <t>Draw a bar plot with the 3 shortest recovery times. Use red color.</t>
   </si>
   <si>
@@ -158,9 +146,6 @@
     <t>Line plot the temperature column, but each value divided by 2</t>
   </si>
   <si>
-    <t>What are the 3 largest yields values?</t>
-  </si>
-  <si>
     <t>geological.xlsx</t>
   </si>
   <si>
@@ -170,24 +155,15 @@
     <t>the biggest depth</t>
   </si>
   <si>
-    <t>pie plot the 3 smallest permeabilities. Add rock type as a legend.</t>
-  </si>
-  <si>
     <t>energy_consumption.xlsx</t>
   </si>
   <si>
-    <t>What are three device ids with the largest usage duration</t>
-  </si>
-  <si>
     <t>Find the correlation between energy cost and power consumption</t>
   </si>
   <si>
     <t>Pie plot 6 usage durations with largest values. State the device ids in the legend</t>
   </si>
   <si>
-    <t>Is there any voltage fluctuation bigger than 3000? Reply Yes or No</t>
-  </si>
-  <si>
     <t>genetics_sic.xlsx</t>
   </si>
   <si>
@@ -197,9 +173,6 @@
     <t>What is the average mutation rate for the rows with protein synthesis rate higher than 228.</t>
   </si>
   <si>
-    <t>Determine the id of a sequence that has the highest gene expression level</t>
-  </si>
-  <si>
     <t>Plot of 4 smallest synthesis rates with title: Report 2021Q1. Place sequence ids on the x axis.</t>
   </si>
   <si>
@@ -212,9 +185,6 @@
     <t>Find the most frequent error code</t>
   </si>
   <si>
-    <t>Barplot top 9 object detection counts. Place robot id on x-axis and set title to Top 9 counts</t>
-  </si>
-  <si>
     <t>Create a scatter plot with voltage on x axis and temperature on y axis</t>
   </si>
   <si>
@@ -224,9 +194,6 @@
     <t>Bar plot of the 7 biggest eps</t>
   </si>
   <si>
-    <t>What is the lowest price</t>
-  </si>
-  <si>
     <t>Add the PE ratio column to the EPS column and find the minimal value of this sum.</t>
   </si>
   <si>
@@ -242,18 +209,12 @@
     <t>Plot the first 10 tissue density values that occur in the table and add their id on x-axis.</t>
   </si>
   <si>
-    <t>Is the average contrast value bigger than the average pixel intensity? Reply Yes or No</t>
-  </si>
-  <si>
     <t>How big is the image processing time for image with id of 27</t>
   </si>
   <si>
     <t>porsche_tmp.xlsx</t>
   </si>
   <si>
-    <t>Identify the model variant with the highest price, along with it’s interior color</t>
-  </si>
-  <si>
     <t>Determine which model variant has the best acceleration.</t>
   </si>
   <si>
@@ -302,24 +263,12 @@
     <t>Filter out the faculties that have less than a 1400 number of students</t>
   </si>
   <si>
-    <t>Identify experiments where the color change had the highest red (R) values separately.</t>
-  </si>
-  <si>
-    <t>What are 5 panel ids with largest power output?</t>
-  </si>
-  <si>
     <t>Plot the average number of male students compared to the average number of female students</t>
   </si>
   <si>
-    <t>Plot the number of international students. Put faculty names to the legend.</t>
-  </si>
-  <si>
     <t>plot the highest unit price and the lowest unit price side by side</t>
   </si>
   <si>
-    <t>Bar plot the torque for each model. Use red color for the plot.</t>
-  </si>
-  <si>
     <t>Plot the frequency of wheel types. Place wheel type on x-axis and the amount of times it occurs on y-axis.</t>
   </si>
   <si>
@@ -357,6 +306,63 @@
   </si>
   <si>
     <t>Calculate the average horsepower-to-weight ratio</t>
+  </si>
+  <si>
+    <t>Identify the experiment where the color change had the highest red (R) values.</t>
+  </si>
+  <si>
+    <t>Determine the pH level most commonly observed across all experiments.</t>
+  </si>
+  <si>
+    <t>covariance between concentration and yield?</t>
+  </si>
+  <si>
+    <t>Scatter plot to visualize the relationship between temperature and reaction time.</t>
+  </si>
+  <si>
+    <t>What are 3 panel ids with largest power output?</t>
+  </si>
+  <si>
+    <t>is there any patient with nausea side effect? If there is, give me the patient's id</t>
+  </si>
+  <si>
+    <t>What is the 3rd largest yield value?</t>
+  </si>
+  <si>
+    <t>pie plot the 3 smallest permeabilities. Add rock types to the legend.</t>
+  </si>
+  <si>
+    <t>boxplot of seismic velocity and density columns</t>
+  </si>
+  <si>
+    <t>What are three device ids with the largest use duration</t>
+  </si>
+  <si>
+    <t>Is there any voltage fluctuation bigger than 3000? Reply yes or no</t>
+  </si>
+  <si>
+    <t>Determine the id of a sequence that has the highest gene expression</t>
+  </si>
+  <si>
+    <t>Barplot 9 biggest object detection counts. Place robot id on x-axis and set title to Top 9 counts</t>
+  </si>
+  <si>
+    <t>What is the second lowest price</t>
+  </si>
+  <si>
+    <t>Is the average contrast value bigger than the average pixel intensity?</t>
+  </si>
+  <si>
+    <t>Identify the model variant with the highest price, along with it’s color</t>
+  </si>
+  <si>
+    <t>Bar plot the torque for each model. Use green color for the plot.</t>
+  </si>
+  <si>
+    <t>What are restock dates from january to april (included)?</t>
+  </si>
+  <si>
+    <t>Pie plot the number of international students. Put faculty names to the legend.</t>
   </si>
 </sst>
 </file>
@@ -755,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15B2F874-D72A-4018-BDE0-E1C1129AFB02}">
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,34 +794,34 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -823,7 +829,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -845,7 +851,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -856,7 +862,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -988,7 +994,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -1021,7 +1027,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -1032,7 +1038,7 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -1043,7 +1049,7 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1054,7 +1060,7 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -1062,10 +1068,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -1073,10 +1079,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C25" t="b">
         <v>1</v>
@@ -1084,10 +1090,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -1095,10 +1101,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
         <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>30</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
@@ -1106,10 +1112,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -1117,10 +1123,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -1128,10 +1134,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -1139,10 +1145,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C31" t="b">
         <v>1</v>
@@ -1150,10 +1156,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
         <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>36</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -1164,7 +1170,7 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -1175,7 +1181,7 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -1186,7 +1192,7 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C35" t="b">
         <v>1</v>
@@ -1197,7 +1203,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -1205,10 +1211,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -1216,10 +1222,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -1227,10 +1233,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="C39" t="b">
         <v>1</v>
@@ -1238,21 +1244,21 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="C40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -1260,32 +1266,32 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -1293,10 +1299,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -1304,10 +1310,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -1315,32 +1321,32 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="C47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -1348,21 +1354,21 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="C51" t="b">
         <v>1</v>
@@ -1370,10 +1376,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C52" t="b">
         <v>1</v>
@@ -1381,43 +1387,43 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -1425,10 +1431,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
@@ -1436,32 +1442,32 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -1469,10 +1475,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
@@ -1480,10 +1486,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -1491,21 +1497,21 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="C63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C64" t="b">
         <v>1</v>
@@ -1513,21 +1519,21 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
@@ -1535,10 +1541,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
@@ -1546,10 +1552,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -1557,10 +1563,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
@@ -1568,43 +1574,43 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B70" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="C70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" t="s">
         <v>76</v>
       </c>
-      <c r="B71" t="s">
-        <v>79</v>
-      </c>
       <c r="C71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B72" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="C72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C73" t="b">
         <v>0</v>
@@ -1612,21 +1618,21 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C74" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
@@ -1634,10 +1640,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
@@ -1645,10 +1651,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B77" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
@@ -1656,41 +1662,63 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B79" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B80" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="C80" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81">
-        <f>COUNTIF(C1:C80,"TRUE")</f>
-        <v>25</v>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81" t="s">
+        <v>75</v>
+      </c>
+      <c r="C81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>69</v>
+      </c>
+      <c r="B82" t="s">
+        <v>108</v>
+      </c>
+      <c r="C82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <f>COUNTIF(C1:C82,"TRUE")</f>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filled up dataset with 82 entities
query, code, prompts, etc.
</commit_message>
<xml_diff>
--- a/dataset/dataset_clean.xlsx
+++ b/dataset/dataset_clean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\micha\homeworks\NLP\AgentToBeNamed\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90FDFE6-86F5-46F4-AA4C-C60BE4D07D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D22549-5F37-4891-9AAB-3817661ECB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{51F2586A-075B-4256-83EE-790A211770F4}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>Create a scatter plot to visualize the relationship between frequency and inductance.</t>
   </si>
   <si>
-    <t>chemicals_1.xlsx</t>
-  </si>
-  <si>
     <t>Histogram of voltage values in the dataset.</t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>genetics_sic.xlsx</t>
   </si>
   <si>
-    <t>Find the most common base pair</t>
-  </si>
-  <si>
     <t>What is the average mutation rate for the rows with protein synthesis rate higher than 228.</t>
   </si>
   <si>
@@ -227,9 +221,6 @@
     <t>skoda_warehouse.xlsx</t>
   </si>
   <si>
-    <t>Identify the part with the highest total value (Total Value = Quantity in Stock * Unit Price).</t>
-  </si>
-  <si>
     <t>Calculate the average quantity in stock for all parts</t>
   </si>
   <si>
@@ -369,6 +360,15 @@
   </si>
   <si>
     <t>code_errors</t>
+  </si>
+  <si>
+    <t>Find the most common base pair sequence</t>
+  </si>
+  <si>
+    <t>Identify the part with the highest total value (total value = quantity in stock * unit price).</t>
+  </si>
+  <si>
+    <t>chemicals.xlsx</t>
   </si>
 </sst>
 </file>
@@ -471,9 +471,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -511,7 +511,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -617,7 +617,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -759,7 +759,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15B2F874-D72A-4018-BDE0-E1C1129AFB02}">
   <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,40 +800,40 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -841,7 +841,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -863,7 +863,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -874,7 +874,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -973,7 +973,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -981,10 +981,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -992,10 +992,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -1003,10 +1003,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -1014,10 +1014,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -1025,10 +1025,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -1036,10 +1036,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -1058,10 +1058,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1069,10 +1069,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -1080,10 +1080,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -1091,10 +1091,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
         <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
       </c>
       <c r="C25" t="b">
         <v>1</v>
@@ -1102,10 +1102,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -1113,10 +1113,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
@@ -1124,10 +1124,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -1135,10 +1135,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>29</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -1146,10 +1146,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" t="b">
         <v>1</v>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -1182,7 +1182,7 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -1193,7 +1193,7 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -1204,7 +1204,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" t="b">
         <v>1</v>
@@ -1215,7 +1215,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
         <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>36</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -1234,10 +1234,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -1245,10 +1245,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C39" t="b">
         <v>1</v>
@@ -1256,10 +1256,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C40" t="b">
         <v>1</v>
@@ -1267,10 +1267,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -1278,10 +1278,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
         <v>38</v>
-      </c>
-      <c r="B42" t="s">
-        <v>39</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -1289,10 +1289,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" t="b">
         <v>1</v>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -1311,10 +1311,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -1322,10 +1322,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
         <v>41</v>
-      </c>
-      <c r="B46" t="s">
-        <v>43</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -1333,10 +1333,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C48" t="b">
         <v>1</v>
@@ -1355,10 +1355,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -1366,10 +1366,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" t="s">
         <v>45</v>
-      </c>
-      <c r="B50" t="s">
-        <v>47</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -1377,10 +1377,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C51" t="b">
         <v>1</v>
@@ -1388,10 +1388,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C52" t="b">
         <v>1</v>
@@ -1399,10 +1399,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C53" t="b">
         <v>1</v>
@@ -1410,10 +1410,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -1421,10 +1421,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C55" t="b">
         <v>1</v>
@@ -1432,10 +1432,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" t="s">
         <v>49</v>
-      </c>
-      <c r="B56" t="s">
-        <v>51</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -1443,10 +1443,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
@@ -1454,10 +1454,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" t="s">
         <v>52</v>
-      </c>
-      <c r="B58" t="s">
-        <v>54</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
@@ -1465,10 +1465,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C59" t="b">
         <v>1</v>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B60" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -1487,10 +1487,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
@@ -1498,10 +1498,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -1509,10 +1509,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B63" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -1520,10 +1520,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C64" t="b">
         <v>1</v>
@@ -1531,10 +1531,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
@@ -1542,10 +1542,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>55</v>
+      </c>
+      <c r="B66" t="s">
         <v>57</v>
-      </c>
-      <c r="B66" t="s">
-        <v>59</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
@@ -1553,10 +1553,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B67" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
@@ -1564,10 +1564,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -1575,10 +1575,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B69" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
@@ -1586,10 +1586,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B70" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
@@ -1597,10 +1597,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C71" t="b">
         <v>1</v>
@@ -1608,10 +1608,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B72" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>60</v>
+      </c>
+      <c r="B73" t="s">
         <v>62</v>
-      </c>
-      <c r="B73" t="s">
-        <v>65</v>
       </c>
       <c r="C73" t="b">
         <v>0</v>
@@ -1630,10 +1630,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B74" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C74" t="b">
         <v>1</v>
@@ -1641,10 +1641,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B75" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
@@ -1652,10 +1652,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B76" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
@@ -1663,10 +1663,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B77" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
@@ -1674,10 +1674,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>65</v>
+      </c>
+      <c r="B78" t="s">
         <v>68</v>
-      </c>
-      <c r="B78" t="s">
-        <v>71</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
@@ -1685,10 +1685,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B79" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C79" t="b">
         <v>0</v>
@@ -1696,10 +1696,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B80" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C80" t="b">
         <v>1</v>
@@ -1707,10 +1707,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B81" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C81" t="b">
         <v>1</v>
@@ -1718,10 +1718,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C82" t="b">
         <v>1</v>

</xml_diff>